<commit_message>
Updated High CCS Storage Cost file, per proposal 129
</commit_message>
<xml_diff>
--- a/Main_User_Workspace/input/energy/ccs/Input Module/CCS Supply Curves.xlsx
+++ b/Main_User_Workspace/input/energy/ccs/Input Module/CCS Supply Curves.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20320" yWindow="0" windowWidth="33600" windowHeight="21420" tabRatio="796" activeTab="1"/>
+    <workbookView xWindow="20200" yWindow="3140" windowWidth="33600" windowHeight="21420" tabRatio="796" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ccs_supply_curves_low" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="933" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="120">
   <si>
     <t>INPUT_TABLE</t>
   </si>
@@ -496,7 +496,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="106">
+  <cellStyleXfs count="108">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -603,6 +603,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -656,7 +658,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="106">
+  <cellStyles count="108">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -709,6 +711,7 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -761,6 +764,7 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="105"/>
   </cellStyles>
@@ -4113,7 +4117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N129"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
@@ -10099,10 +10103,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -10167,7 +10171,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="24">
-        <v>2020</v>
+        <v>1975</v>
       </c>
       <c r="F6" s="24">
         <v>10000</v>
@@ -10187,7 +10191,7 @@
         <v>9</v>
       </c>
       <c r="E7" s="24">
-        <v>2035</v>
+        <v>1990</v>
       </c>
       <c r="F7" s="24">
         <v>10000</v>
@@ -10207,7 +10211,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="24">
-        <v>2050</v>
+        <v>2005</v>
       </c>
       <c r="F8" s="24">
         <v>10000</v>
@@ -10227,7 +10231,7 @@
         <v>9</v>
       </c>
       <c r="E9" s="24">
-        <v>2065</v>
+        <v>2020</v>
       </c>
       <c r="F9" s="24">
         <v>10000</v>
@@ -10247,7 +10251,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="24">
-        <v>2080</v>
+        <v>2035</v>
       </c>
       <c r="F10" s="24">
         <v>10000</v>
@@ -10267,14 +10271,255 @@
         <v>9</v>
       </c>
       <c r="E11" s="24">
+        <v>2050</v>
+      </c>
+      <c r="F11" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="24">
+        <v>2065</v>
+      </c>
+      <c r="F12" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="24">
+        <v>2080</v>
+      </c>
+      <c r="F13" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="24">
         <v>2095</v>
       </c>
-      <c r="F11" s="24">
+      <c r="F14" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="24">
+        <v>1975</v>
+      </c>
+      <c r="F15" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="24">
+        <v>1990</v>
+      </c>
+      <c r="F16" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="24">
+        <v>2005</v>
+      </c>
+      <c r="F17" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="24">
+        <v>2020</v>
+      </c>
+      <c r="F18" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="24">
+        <v>2035</v>
+      </c>
+      <c r="F19" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20" s="24">
+        <v>2050</v>
+      </c>
+      <c r="F20" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="24">
+        <v>2065</v>
+      </c>
+      <c r="F21" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E22" s="24">
+        <v>2080</v>
+      </c>
+      <c r="F22" s="24">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="24">
+        <v>2095</v>
+      </c>
+      <c r="F23" s="24">
         <v>10000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>